<commit_message>
cleaned repo from old files
</commit_message>
<xml_diff>
--- a/RCSdata/data/deriv_compounds_properties.xlsx
+++ b/RCSdata/data/deriv_compounds_properties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,34 +441,34 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>underiv_comp_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>iupac_name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>molecular_formula</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>canonical_smiles</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>molecular_weight</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>xlogp</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>underiv_comp_name</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>el_C</t>
@@ -567,66 +567,61 @@
       <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>fg_mf_ketone</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>fg_mf_total</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>myristic acid, tms derivative</t>
+          <t>stearic acid, tms derivative</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>stearic acid</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C14H28O2</t>
+          <t>octadecanoic acid</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>228.37</v>
+          <t>C18H36O2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>myristic acid</t>
-        </is>
+        <v>284.5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7.4</v>
       </c>
       <c r="H2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I2" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J2" t="n">
         <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7363226343214958</v>
+        <v>0.7599226713532512</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1235889127293427</v>
+        <v>0.1275500878734622</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1401147261023777</v>
+        <v>0.1124710017574693</v>
       </c>
       <c r="N2" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -647,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8029031834303979</v>
+        <v>0.8417117750439367</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -656,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>0.1971230897228183</v>
+        <v>0.1582319859402461</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -666,72 +661,69 @@
       </c>
       <c r="AA2" t="n">
         <v>0</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>palmitelaidic acid, tms derivative</t>
+          <t>benzene-1,2-diol, deriv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(e)-hexadec-9-enoic acid</t>
+          <t>benzene-1,2-diol</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C16H30O2</t>
+          <t>benzene-1,2-diol</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CCCCCCC=CCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>254.41</v>
+          <t>C6H6O2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>C1=CC=C(C(=C1)O)O</t>
+        </is>
       </c>
       <c r="F3" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>palmitelaidic acid</t>
-        </is>
+        <v>110.11</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9</v>
       </c>
       <c r="H3" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="I3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7553791124562713</v>
+        <v>0.6544909635818728</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1188632522306513</v>
+        <v>0.05492689129052766</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1257733579654888</v>
+        <v>0.2906003087821269</v>
       </c>
       <c r="N3" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -743,16 +735,16 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8230690617507173</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>0.6911088911088911</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>0.3089092725456362</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1769466609016941</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
@@ -762,76 +754,73 @@
       </c>
       <c r="AA3" t="n">
         <v>0</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>palmitic acid, tms derivative</t>
+          <t>1-monopalmitin, 2tms derivative</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>1-monopalmitin</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>2,3-dihydroxypropyl hexadecanoate</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>256.42</v>
+          <t>C19H38O4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCCCC(=O)OCC(CO)O</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>palmitic acid</t>
-        </is>
+        <v>330.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.3</v>
       </c>
       <c r="H4" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I4" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.6904962178517398</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.1158971255673222</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.1936338880484115</v>
+      </c>
+      <c r="N4" t="n">
+        <v>17</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
         <v>2</v>
       </c>
-      <c r="K4" t="n">
-        <v>0.7494579205990172</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.125793619842446</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.1247874580765931</v>
-      </c>
-      <c r="N4" t="n">
-        <v>15</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
       <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>1</v>
       </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
@@ -839,95 +828,92 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8244793697839481</v>
+        <v>0.7215098335854766</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>0.1029167927382754</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>0.1756006051437216</v>
       </c>
       <c r="Z4" t="n">
         <v>0</v>
       </c>
       <c r="AA4" t="n">
         <v>0</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>9,12-octadecadienoic acid (z,z)-, tms derivative</t>
+          <t>1-monooleoylglycerol, 2tms derivative</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>1-monooleoylglycerol</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>2,3-dihydroxypropyl (z)-octadec-9-enoate</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>280.4</v>
+          <t>C21H40O4</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)OCC(CO)O</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>9,12-octadecadienoic acid (z,z)-</t>
-        </is>
+        <v>356.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6.5</v>
       </c>
       <c r="H5" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I5" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.7075203366058906</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.1130995792426367</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1795119214586255</v>
+      </c>
+      <c r="N5" t="n">
+        <v>19</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>2</v>
       </c>
-      <c r="K5" t="n">
-        <v>0.7710342368045648</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.1150356633380885</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.1141155492154066</v>
-      </c>
-      <c r="N5" t="n">
-        <v>17</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
       <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
         <v>1</v>
       </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
@@ -935,61 +921,58 @@
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8396398002853066</v>
+        <v>0.7419270687237027</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>0.09541093969144461</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>0.1627938288920056</v>
       </c>
       <c r="Z5" t="n">
         <v>0</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>oleic acid, tms derivative</t>
+          <t>9-octadecenoic acid, (e)-, deriv</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>9-octadecenoic acid, (e)-</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>(e)-octadec-9-enoic acid</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>C18H34O2</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>282.5</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>6.5</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>oleic acid</t>
-        </is>
       </c>
       <c r="H6" t="n">
         <v>18</v>
@@ -1050,15 +1033,12 @@
       </c>
       <c r="AA6" t="n">
         <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>stearic acid, tms derivative</t>
+          <t>octadecanoic acid, deriv</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1068,24 +1048,24 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>octadecanoic acid</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>C18H36O2</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>CCCCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>284.5</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>7.4</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>stearic acid</t>
-        </is>
       </c>
       <c r="H7" t="n">
         <v>18</v>
@@ -1146,60 +1126,57 @@
       </c>
       <c r="AA7" t="n">
         <v>0</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>1-monopalmitin, 2tms derivative</t>
+          <t>9,12-octadecadienoic acid (z,z)-, tms derivative</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2,3-dihydroxypropyl hexadecanoate</t>
+          <t>9,12-octadecadienoic acid (z,z)-</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C19H38O4</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)OCC(CO)O</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>330.5</v>
+          <t>C18H32O2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F8" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>1-monopalmitin</t>
-        </is>
+        <v>280.4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6.8</v>
       </c>
       <c r="H8" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6904962178517398</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1158971255673222</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1936338880484115</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="N8" t="n">
         <v>17</v>
@@ -1208,13 +1185,13 @@
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1223,28 +1200,25 @@
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.7215098335854766</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="V8" t="n">
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.1029167927382754</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.1756006051437216</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
       </c>
       <c r="AA8" t="n">
         <v>0</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="9">
@@ -1255,29 +1229,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>1-monolinolein</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>2,3-dihydroxypropyl (9z,12z)-octadeca-9,12-dienoate</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>C21H38O4</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>CCCCCC=CCC=CCCCCCCCC(=O)OCC(CO)O</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>354.5</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>5.8</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1-monolinolein</t>
-        </is>
       </c>
       <c r="H9" t="n">
         <v>21</v>
@@ -1338,75 +1312,72 @@
       </c>
       <c r="AA9" t="n">
         <v>0</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>1-monooleoylglycerol, 2tms derivative</t>
+          <t>tetradecanoic acid, deriv</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2,3-dihydroxypropyl (z)-octadec-9-enoate</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C21H40O4</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)OCC(CO)O</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>356.5</v>
+          <t>C14H28O2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F10" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1-monooleoylglycerol</t>
-        </is>
+        <v>228.37</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5.3</v>
       </c>
       <c r="H10" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I10" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="J10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7075203366058906</v>
+        <v>0.7363226343214958</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1130995792426367</v>
+        <v>0.1235889127293427</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1795119214586255</v>
+        <v>0.1401147261023777</v>
       </c>
       <c r="N10" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1415,181 +1386,175 @@
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>0.7419270687237027</v>
+        <v>0.8029031834303979</v>
       </c>
       <c r="V10" t="n">
         <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>0.09541093969144461</v>
+        <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>0.1971230897228183</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1627938288920056</v>
+        <v>0</v>
       </c>
       <c r="Z10" t="n">
         <v>0</v>
       </c>
       <c r="AA10" t="n">
         <v>0</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>glycerol monostearate, 2tms derivative</t>
+          <t>4-oxopentanoic acid, deriv</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2,3-dihydroxypropyl octadecanoate</t>
+          <t>4-oxopentanoic acid</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C21H42O4</t>
+          <t>4-oxopentanoic acid</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCCCC(=O)OCC(CO)O</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>358.6</v>
+          <t>C5H8O3</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CC(=O)CCC(=O)O</t>
+        </is>
       </c>
       <c r="F11" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>glycerol monostearate</t>
-        </is>
+        <v>116.11</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.5</v>
       </c>
       <c r="H11" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="J11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7033770217512548</v>
+        <v>0.5172250452157436</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1180591187953151</v>
+        <v>0.06945138230987856</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1784606804238706</v>
+        <v>0.413375247610025</v>
       </c>
       <c r="N11" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
         <v>1</v>
       </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0</v>
-      </c>
       <c r="U11" t="n">
-        <v>0.7432041271611823</v>
+        <v>0.1208078546206184</v>
       </c>
       <c r="V11" t="n">
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>0.09485220301171221</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>0</v>
+        <v>0.3877099302385669</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.161840490797546</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="n">
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>1.00004342790967</v>
+        <v>0.491533890276462</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>benzoic acid, deriv.</t>
+          <t>palmitic acid, tms derivative</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>benzoic acid</t>
+          <t>palmitic acid</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C7H6O2</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)C(=O)O</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>122.12</v>
+          <t>C16H32O2</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F12" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>benzoic acid</t>
-        </is>
+        <v>256.42</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6.4</v>
       </c>
       <c r="H12" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I12" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="J12" t="n">
         <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>0.6884785456927611</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L12" t="n">
-        <v>0.04952505732066819</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2620209629872257</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -1607,16 +1572,16 @@
         <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="V12" t="n">
-        <v>0.6313953488372093</v>
+        <v>0</v>
       </c>
       <c r="W12" t="n">
         <v>0</v>
       </c>
       <c r="X12" t="n">
-        <v>0.3686292171634458</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -1626,63 +1591,60 @@
       </c>
       <c r="AA12" t="n">
         <v>0</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>tetradecanoic acid, deriv.</t>
+          <t>hexadecanoic acid, deriv</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C14H28O2</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>228.37</v>
+          <t>C16H32O2</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F13" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>tetradecanoic acid</t>
-        </is>
+        <v>256.42</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6.4</v>
       </c>
       <c r="H13" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I13" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J13" t="n">
         <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7363226343214958</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1235889127293427</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1401147261023777</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="N13" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
@@ -1703,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>0.8029031834303979</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="V13" t="n">
         <v>0</v>
@@ -1712,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1971230897228183</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -1722,168 +1684,162 @@
       </c>
       <c r="AA13" t="n">
         <v>0</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>hexadecanoic acid, deriv.</t>
+          <t>2-methoxy-4-methylphenol, deriv</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>2-methoxy-4-methylphenol</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>2-methoxy-4-methylphenol</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>256.42</v>
+          <t>C8H10O2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>CC1=CC(=C(C=C1)O)OC</t>
+        </is>
       </c>
       <c r="F14" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>hexadecanoic acid</t>
-        </is>
+        <v>138.16</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.3</v>
       </c>
       <c r="H14" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I14" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="J14" t="n">
         <v>2</v>
       </c>
       <c r="K14" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.6954834973943254</v>
       </c>
       <c r="L14" t="n">
-        <v>0.125793619842446</v>
+        <v>0.07295888824551246</v>
       </c>
       <c r="M14" t="n">
-        <v>0.1247874580765931</v>
+        <v>0.2316010422698321</v>
       </c>
       <c r="N14" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
         <v>1</v>
       </c>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
       <c r="T14" t="n">
         <v>0</v>
       </c>
       <c r="U14" t="n">
-        <v>0.8244793697839481</v>
+        <v>0.1088231036479444</v>
       </c>
       <c r="V14" t="n">
-        <v>0</v>
+        <v>0.4565648523451071</v>
       </c>
       <c r="W14" t="n">
-        <v>0</v>
+        <v>0.1230964099594673</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>0.3115590619571512</v>
       </c>
       <c r="AA14" t="n">
         <v>0</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid, deriv.</t>
+          <t>2,4-dimethylphenol, deriv</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>2,4-dimethylphenol</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>2,4-dimethylphenol</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>280.4</v>
+          <t>C8H10O</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CC1=CC(=C(C=C1)O)C</t>
+        </is>
       </c>
       <c r="F15" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
-        </is>
+        <v>122.16</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.3</v>
       </c>
       <c r="H15" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I15" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.7865749836280288</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0825147347740668</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.1309675834970531</v>
+      </c>
+      <c r="N15" t="n">
         <v>2</v>
       </c>
-      <c r="K15" t="n">
-        <v>0.7710342368045648</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.1150356633380885</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.1141155492154066</v>
-      </c>
-      <c r="N15" t="n">
-        <v>17</v>
-      </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" t="n">
         <v>0</v>
@@ -1895,16 +1851,16 @@
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>0.8396398002853066</v>
+        <v>0.2461525867714473</v>
       </c>
       <c r="V15" t="n">
-        <v>0</v>
+        <v>0.6146856581532416</v>
       </c>
       <c r="W15" t="n">
-        <v>0</v>
+        <v>0.1392190569744597</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="n">
         <v>0</v>
@@ -1914,63 +1870,60 @@
       </c>
       <c r="AA15" t="n">
         <v>0</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>9-octadecenoic acid, (e)-, deriv.</t>
+          <t>palmitelaidic acid, tms derivative</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>(e)-octadec-9-enoic acid</t>
+          <t>palmitelaidic acid</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>(e)-hexadec-9-enoic acid</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>282.5</v>
+          <t>C16H30O2</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CCCCCCC=CCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F16" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>9-octadecenoic acid, (e)-</t>
-        </is>
+        <v>254.41</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6.4</v>
       </c>
       <c r="H16" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I16" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J16" t="n">
         <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.7553791124562713</v>
       </c>
       <c r="L16" t="n">
-        <v>0.121316814159292</v>
+        <v>0.1188632522306513</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.1257733579654888</v>
       </c>
       <c r="N16" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
@@ -1991,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="U16" t="n">
-        <v>0.8405345132743363</v>
+        <v>0.8230690617507173</v>
       </c>
       <c r="V16" t="n">
         <v>0</v>
@@ -2000,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>0.1593522123893805</v>
+        <v>0.1769466609016941</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
@@ -2010,60 +1963,57 @@
       </c>
       <c r="AA16" t="n">
         <v>0</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>octadecanoic acid, deriv.</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid, deriv</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>octadecanoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C18H36O2</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCCCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>284.5</v>
+          <t>C18H32O2</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F17" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>octadecanoic acid</t>
-        </is>
+        <v>280.4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6.8</v>
       </c>
       <c r="H17" t="n">
         <v>18</v>
       </c>
       <c r="I17" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J17" t="n">
         <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7599226713532512</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1275500878734622</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="M17" t="n">
-        <v>0.1124710017574693</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="N17" t="n">
         <v>17</v>
@@ -2087,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>0.8417117750439367</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="V17" t="n">
         <v>0</v>
@@ -2096,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>0.1582319859402461</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="Y17" t="n">
         <v>0</v>
@@ -2106,73 +2056,70 @@
       </c>
       <c r="AA17" t="n">
         <v>0</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>phenol, deriv.</t>
+          <t>myristic acid, tms derivative</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>myristic acid</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>94.11</v>
+          <t>C14H28O2</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F18" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>phenol</t>
-        </is>
+        <v>228.37</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5.3</v>
       </c>
       <c r="H18" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I18" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="J18" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.7363226343214958</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.1235889127293427</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.1401147261023777</v>
+      </c>
+      <c r="N18" t="n">
+        <v>13</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
         <v>1</v>
       </c>
-      <c r="K18" t="n">
-        <v>0.765763468281798</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.06426522154925088</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.1700031877590054</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>6</v>
-      </c>
-      <c r="P18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
@@ -2183,16 +2130,16 @@
         <v>0</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
+        <v>0.8029031834303979</v>
       </c>
       <c r="V18" t="n">
-        <v>0.8193178195728402</v>
+        <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>0.1971230897228183</v>
       </c>
       <c r="Y18" t="n">
         <v>0</v>
@@ -2202,72 +2149,69 @@
       </c>
       <c r="AA18" t="n">
         <v>0</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>4-oxopentanoic acid, deriv.</t>
+          <t>phenol, deriv</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4-oxopentanoic acid</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>C5H8O3</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CC(=O)CCC(=O)O</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>116.11</v>
+          <t>C6H6O</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>C1=CC=C(C=C1)O</t>
+        </is>
       </c>
       <c r="F19" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>4-oxopentanoic acid</t>
-        </is>
+        <v>94.11</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.5</v>
       </c>
       <c r="H19" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I19" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>0.5172250452157436</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="L19" t="n">
-        <v>0.06945138230987856</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="M19" t="n">
-        <v>0.413375247610025</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>6</v>
+      </c>
+      <c r="P19" t="n">
         <v>1</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
       <c r="Q19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" t="n">
         <v>0</v>
@@ -2276,19 +2220,19 @@
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" t="n">
-        <v>0.1208078546206184</v>
+        <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>0</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
       <c r="X19" t="n">
-        <v>0.3877099302385669</v>
+        <v>0</v>
       </c>
       <c r="Y19" t="n">
         <v>0</v>
@@ -2297,67 +2241,64 @@
         <v>0</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.491533890276462</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>1.00004342790967</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>benzene-1,2-diol, deriv.</t>
+          <t>glycerol monostearate, 2tms derivative</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>benzene-1,2-diol</t>
+          <t>glycerol monostearate</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>C6H6O2</t>
+          <t>2,3-dihydroxypropyl octadecanoate</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>C1=CC=C(C(=C1)O)O</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>110.11</v>
+          <t>C21H42O4</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CCCCCCCCCCCCCCCCCC(=O)OCC(CO)O</t>
+        </is>
       </c>
       <c r="F20" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>benzene-1,2-diol</t>
-        </is>
+        <v>358.6</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.4</v>
       </c>
       <c r="H20" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="I20" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K20" t="n">
-        <v>0.6544909635818728</v>
+        <v>0.7033770217512548</v>
       </c>
       <c r="L20" t="n">
-        <v>0.05492689129052766</v>
+        <v>0.1180591187953151</v>
       </c>
       <c r="M20" t="n">
-        <v>0.2906003087821269</v>
+        <v>0.1784606804238706</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O20" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
         <v>2</v>
@@ -2366,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -2375,92 +2316,89 @@
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>0</v>
+        <v>0.7432041271611823</v>
       </c>
       <c r="V20" t="n">
-        <v>0.6911088911088911</v>
+        <v>0</v>
       </c>
       <c r="W20" t="n">
-        <v>0.3089092725456362</v>
+        <v>0.09485220301171221</v>
       </c>
       <c r="X20" t="n">
         <v>0</v>
       </c>
       <c r="Y20" t="n">
-        <v>0</v>
+        <v>0.161840490797546</v>
       </c>
       <c r="Z20" t="n">
         <v>0</v>
       </c>
       <c r="AA20" t="n">
         <v>0</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2,4-dimethylphenol, deriv.</t>
+          <t>oleic acid, tms derivative</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2,4-dimethylphenol</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>C8H10O</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CC1=CC(=C(C=C1)O)C</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>122.16</v>
+          <t>C18H34O2</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+        </is>
       </c>
       <c r="F21" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2,4-dimethylphenol</t>
-        </is>
+        <v>282.5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>6.5</v>
       </c>
       <c r="H21" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I21" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="J21" t="n">
+        <v>2</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.7653026548672566</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.121316814159292</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.1132672566371681</v>
+      </c>
+      <c r="N21" t="n">
+        <v>17</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
         <v>1</v>
       </c>
-      <c r="K21" t="n">
-        <v>0.7865749836280288</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0.0825147347740668</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0.1309675834970531</v>
-      </c>
-      <c r="N21" t="n">
-        <v>2</v>
-      </c>
-      <c r="O21" t="n">
-        <v>6</v>
-      </c>
-      <c r="P21" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
       <c r="R21" t="n">
         <v>0</v>
       </c>
@@ -2471,16 +2409,16 @@
         <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>0.2461525867714473</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="V21" t="n">
-        <v>0.6146856581532416</v>
+        <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>0.1392190569744597</v>
+        <v>0</v>
       </c>
       <c r="X21" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="Y21" t="n">
         <v>0</v>
@@ -2490,105 +2428,99 @@
       </c>
       <c r="AA21" t="n">
         <v>0</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2-methoxy-4-methylphenol, deriv.</t>
+          <t>benzoic acid, deriv</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2-methoxy-4-methylphenol</t>
+          <t>benzoic acid</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>C8H10O2</t>
+          <t>benzoic acid</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>CC1=CC(=C(C=C1)O)OC</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>138.16</v>
+          <t>C7H6O2</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>C1=CC=C(C=C1)C(=O)O</t>
+        </is>
       </c>
       <c r="F22" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2-methoxy-4-methylphenol</t>
-        </is>
+        <v>122.12</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.9</v>
       </c>
       <c r="H22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I22" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J22" t="n">
         <v>2</v>
       </c>
       <c r="K22" t="n">
-        <v>0.6954834973943254</v>
+        <v>0.6884785456927611</v>
       </c>
       <c r="L22" t="n">
-        <v>0.07295888824551246</v>
+        <v>0.04952505732066819</v>
       </c>
       <c r="M22" t="n">
-        <v>0.2316010422698321</v>
+        <v>0.2620209629872257</v>
       </c>
       <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>6</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
         <v>1</v>
       </c>
-      <c r="O22" t="n">
-        <v>5</v>
-      </c>
-      <c r="P22" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
       <c r="R22" t="n">
         <v>0</v>
       </c>
       <c r="S22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22" t="n">
         <v>0</v>
       </c>
       <c r="U22" t="n">
-        <v>0.1088231036479444</v>
+        <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>0.4565648523451071</v>
+        <v>0.6313953488372093</v>
       </c>
       <c r="W22" t="n">
-        <v>0.1230964099594673</v>
+        <v>0</v>
       </c>
       <c r="X22" t="n">
-        <v>0</v>
+        <v>0.3686292171634458</v>
       </c>
       <c r="Y22" t="n">
         <v>0</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.3115590619571512</v>
+        <v>0</v>
       </c>
       <c r="AA22" t="n">
         <v>0</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>1.00004342790967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>